<commit_message>
updating arc-ic price dataset
</commit_message>
<xml_diff>
--- a/data-raw/fsaArcPlc/input_data/fsaArcIcPrice/ARC_IC_2023.xlsx
+++ b/data-raw/fsaArcPlc/input_data/fsaArcIcPrice/ARC_IC_2023.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28227"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\EPAS\2014FBIMP\ARC_PLC\Webpage Posting\2024-0208\Program Year 2023\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\EPAS\2014FBIMP\ARC_PLC\Webpage Posting\2025-0131\Program Year 2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4482F762-AB06-49E8-80F9-FE10ABDDE921}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A999505-0800-41D8-BF69-4EC870106F3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ARC_IC BM Prices" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="75">
   <si>
     <t>TABLE 5.  2023 BENCHMARK AND ACTUAL PRICE CALCULATIONS FOR INDIVIDUAL AGRICULTURAL RISK COVERAGE (ARC-IC)</t>
   </si>
@@ -28,7 +28,7 @@
     <t>BASED ON 2017/18-2021/22 MARKET YEAR AVERAGE (MYA) PRICES AND EFFECTIVE REFERENCE PRICES</t>
   </si>
   <si>
-    <t>February 8, 2024 1/</t>
+    <t>January 31, 2025 1/</t>
   </si>
   <si>
     <t>Commodity</t>
@@ -82,7 +82,7 @@
     <t>Bushel</t>
   </si>
   <si>
-    <t>P</t>
+    <t>F</t>
   </si>
   <si>
     <t>Barley</t>
@@ -215,9 +215,6 @@
   </si>
   <si>
     <t>E</t>
-  </si>
-  <si>
-    <t>F</t>
   </si>
   <si>
     <t>G</t>
@@ -254,10 +251,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
-    <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.000"/>
-    <numFmt numFmtId="166" formatCode="&quot;$&quot;#,##0.0000"/>
+    <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.0000"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -520,7 +516,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -569,25 +565,7 @@
     <xf numFmtId="165" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="2" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="2" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -596,16 +574,16 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="2" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="2" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="2" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="2" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="2" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="2" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="2" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="2" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -811,187 +789,187 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
-      <c r="J1" s="31"/>
-      <c r="K1" s="31"/>
-      <c r="L1" s="31"/>
-      <c r="M1" s="31"/>
-      <c r="N1" s="31"/>
-      <c r="O1" s="31"/>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
+      <c r="K1" s="25"/>
+      <c r="L1" s="25"/>
+      <c r="M1" s="25"/>
+      <c r="N1" s="25"/>
+      <c r="O1" s="25"/>
     </row>
     <row r="2" spans="1:15" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="30" t="s">
+      <c r="A2" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="31"/>
-      <c r="C2" s="31"/>
-      <c r="D2" s="31"/>
-      <c r="E2" s="31"/>
-      <c r="F2" s="31"/>
-      <c r="G2" s="31"/>
-      <c r="H2" s="31"/>
-      <c r="I2" s="31"/>
-      <c r="J2" s="31"/>
-      <c r="K2" s="31"/>
-      <c r="L2" s="31"/>
-      <c r="M2" s="31"/>
-      <c r="N2" s="31"/>
-      <c r="O2" s="31"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="25"/>
+      <c r="I2" s="25"/>
+      <c r="J2" s="25"/>
+      <c r="K2" s="25"/>
+      <c r="L2" s="25"/>
+      <c r="M2" s="25"/>
+      <c r="N2" s="25"/>
+      <c r="O2" s="25"/>
     </row>
     <row r="3" spans="1:15" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="30" t="s">
+      <c r="A3" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="31"/>
-      <c r="C3" s="31"/>
-      <c r="D3" s="31"/>
-      <c r="E3" s="31"/>
-      <c r="F3" s="31"/>
-      <c r="G3" s="31"/>
-      <c r="H3" s="31"/>
-      <c r="I3" s="31"/>
-      <c r="J3" s="31"/>
-      <c r="K3" s="31"/>
-      <c r="L3" s="31"/>
-      <c r="M3" s="31"/>
-      <c r="N3" s="31"/>
-      <c r="O3" s="31"/>
+      <c r="B3" s="25"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="25"/>
+      <c r="H3" s="25"/>
+      <c r="I3" s="25"/>
+      <c r="J3" s="25"/>
+      <c r="K3" s="25"/>
+      <c r="L3" s="25"/>
+      <c r="M3" s="25"/>
+      <c r="N3" s="25"/>
+      <c r="O3" s="25"/>
     </row>
     <row r="5" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A5" s="38" t="s">
+      <c r="A5" s="32" t="s">
         <v>60</v>
       </c>
-      <c r="B5" s="39" t="s">
+      <c r="B5" s="33" t="s">
         <v>61</v>
       </c>
-      <c r="C5" s="39" t="s">
+      <c r="C5" s="33" t="s">
         <v>62</v>
       </c>
-      <c r="D5" s="39" t="s">
+      <c r="D5" s="33" t="s">
         <v>63</v>
       </c>
-      <c r="E5" s="39" t="s">
+      <c r="E5" s="33" t="s">
         <v>64</v>
       </c>
-      <c r="F5" s="39" t="s">
+      <c r="F5" s="33" t="s">
+        <v>20</v>
+      </c>
+      <c r="G5" s="33" t="s">
         <v>65</v>
       </c>
-      <c r="G5" s="39" t="s">
+      <c r="H5" s="33" t="s">
         <v>66</v>
       </c>
-      <c r="H5" s="39" t="s">
+      <c r="I5" s="33" t="s">
         <v>67</v>
       </c>
-      <c r="I5" s="39" t="s">
+      <c r="J5" s="33" t="s">
         <v>68</v>
       </c>
-      <c r="J5" s="39" t="s">
+      <c r="K5" s="33" t="s">
         <v>69</v>
       </c>
-      <c r="K5" s="39" t="s">
+      <c r="L5" s="33"/>
+      <c r="M5" s="33" t="s">
         <v>70</v>
       </c>
-      <c r="L5" s="39"/>
-      <c r="M5" s="39" t="s">
+      <c r="N5" s="33" t="s">
         <v>71</v>
       </c>
-      <c r="N5" s="39" t="s">
+      <c r="O5" s="33"/>
+    </row>
+    <row r="6" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A6" s="34"/>
+      <c r="B6" s="35"/>
+      <c r="C6" s="35"/>
+      <c r="D6" s="35"/>
+      <c r="E6" s="35"/>
+      <c r="F6" s="35"/>
+      <c r="G6" s="35"/>
+      <c r="H6" s="35"/>
+      <c r="I6" s="35"/>
+      <c r="J6" s="35"/>
+      <c r="K6" s="36"/>
+      <c r="L6" s="36"/>
+      <c r="M6" s="35"/>
+      <c r="N6" s="37" t="s">
         <v>72</v>
       </c>
-      <c r="O5" s="39"/>
-    </row>
-    <row r="6" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A6" s="40"/>
-      <c r="B6" s="41"/>
-      <c r="C6" s="41"/>
-      <c r="D6" s="41"/>
-      <c r="E6" s="41"/>
-      <c r="F6" s="41"/>
-      <c r="G6" s="41"/>
-      <c r="H6" s="41"/>
-      <c r="I6" s="41"/>
-      <c r="J6" s="41"/>
-      <c r="K6" s="42"/>
-      <c r="L6" s="42"/>
-      <c r="M6" s="41"/>
-      <c r="N6" s="43" t="s">
+      <c r="O6" s="36"/>
+    </row>
+    <row r="7" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A7" s="30" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="31" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="31" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7" s="31" t="s">
+        <v>7</v>
+      </c>
+      <c r="F7" s="38" t="s">
         <v>73</v>
       </c>
-      <c r="O6" s="42"/>
-    </row>
-    <row r="7" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A7" s="36" t="s">
-        <v>3</v>
-      </c>
-      <c r="B7" s="37" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" s="37" t="s">
-        <v>5</v>
-      </c>
-      <c r="D7" s="37" t="s">
-        <v>6</v>
-      </c>
-      <c r="E7" s="37" t="s">
-        <v>7</v>
-      </c>
-      <c r="F7" s="44" t="s">
+      <c r="G7" s="38"/>
+      <c r="H7" s="38"/>
+      <c r="I7" s="38"/>
+      <c r="J7" s="38"/>
+      <c r="K7" s="38" t="s">
         <v>74</v>
       </c>
-      <c r="G7" s="44"/>
-      <c r="H7" s="44"/>
-      <c r="I7" s="44"/>
-      <c r="J7" s="44"/>
-      <c r="K7" s="44" t="s">
-        <v>75</v>
-      </c>
-      <c r="L7" s="44"/>
-      <c r="M7" s="44"/>
-      <c r="N7" s="44"/>
-      <c r="O7" s="44"/>
+      <c r="L7" s="38"/>
+      <c r="M7" s="38"/>
+      <c r="N7" s="38"/>
+      <c r="O7" s="38"/>
     </row>
     <row r="8" spans="1:15" ht="75.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="33"/>
-      <c r="B8" s="34"/>
-      <c r="C8" s="34"/>
-      <c r="D8" s="34"/>
-      <c r="E8" s="34"/>
-      <c r="F8" s="35" t="s">
+      <c r="A8" s="27"/>
+      <c r="B8" s="28"/>
+      <c r="C8" s="28"/>
+      <c r="D8" s="28"/>
+      <c r="E8" s="28"/>
+      <c r="F8" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="G8" s="35" t="s">
+      <c r="G8" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="H8" s="35" t="s">
+      <c r="H8" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="I8" s="35" t="s">
+      <c r="I8" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="J8" s="35" t="s">
+      <c r="J8" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="K8" s="34" t="s">
+      <c r="K8" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="L8" s="34"/>
-      <c r="M8" s="35" t="s">
+      <c r="L8" s="28"/>
+      <c r="M8" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="N8" s="34" t="s">
+      <c r="N8" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="O8" s="34"/>
+      <c r="O8" s="28"/>
     </row>
     <row r="9" spans="1:15" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
@@ -1025,7 +1003,7 @@
         <v>7.63</v>
       </c>
       <c r="K9" s="7">
-        <v>7.2</v>
+        <v>6.96</v>
       </c>
       <c r="L9" s="8" t="s">
         <v>20</v>
@@ -1034,7 +1012,7 @@
         <v>3.38</v>
       </c>
       <c r="N9" s="7">
-        <v>7.2</v>
+        <v>6.96</v>
       </c>
       <c r="O9" s="8" t="s">
         <v>20</v>
@@ -1072,7 +1050,7 @@
         <v>5.31</v>
       </c>
       <c r="K10" s="7">
-        <v>7.5</v>
+        <v>7.39</v>
       </c>
       <c r="L10" s="8" t="s">
         <v>20</v>
@@ -1081,7 +1059,7 @@
         <v>2.5</v>
       </c>
       <c r="N10" s="7">
-        <v>7.5</v>
+        <v>7.39</v>
       </c>
       <c r="O10" s="8" t="s">
         <v>20</v>
@@ -1119,7 +1097,7 @@
         <v>4.55</v>
       </c>
       <c r="K11" s="7">
-        <v>3.7</v>
+        <v>3.92</v>
       </c>
       <c r="L11" s="8" t="s">
         <v>20</v>
@@ -1128,7 +1106,7 @@
         <v>2</v>
       </c>
       <c r="N11" s="7">
-        <v>3.7</v>
+        <v>3.92</v>
       </c>
       <c r="O11" s="8" t="s">
         <v>20</v>
@@ -1166,7 +1144,7 @@
         <v>0.26750000000000002</v>
       </c>
       <c r="K12" s="14">
-        <v>0.27500000000000002</v>
+        <v>0.26900000000000002</v>
       </c>
       <c r="L12" s="8" t="s">
         <v>20</v>
@@ -1175,7 +1153,7 @@
         <v>0.17749999999999999</v>
       </c>
       <c r="N12" s="14">
-        <v>0.27500000000000002</v>
+        <v>0.26900000000000002</v>
       </c>
       <c r="O12" s="8" t="s">
         <v>20</v>
@@ -1213,7 +1191,7 @@
         <v>6</v>
       </c>
       <c r="K13" s="7">
-        <v>4.8</v>
+        <v>4.55</v>
       </c>
       <c r="L13" s="8" t="s">
         <v>20</v>
@@ -1222,7 +1200,7 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="N13" s="7">
-        <v>4.8</v>
+        <v>4.55</v>
       </c>
       <c r="O13" s="8" t="s">
         <v>20</v>
@@ -1260,7 +1238,7 @@
         <v>5.94</v>
       </c>
       <c r="K14" s="7">
-        <v>4.8499999999999996</v>
+        <v>4.93</v>
       </c>
       <c r="L14" s="8" t="s">
         <v>20</v>
@@ -1269,7 +1247,7 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="N14" s="7">
-        <v>4.8499999999999996</v>
+        <v>4.93</v>
       </c>
       <c r="O14" s="8" t="s">
         <v>20</v>
@@ -1307,7 +1285,7 @@
         <v>13.3</v>
       </c>
       <c r="K15" s="7">
-        <v>12.65</v>
+        <v>12.4</v>
       </c>
       <c r="L15" s="8" t="s">
         <v>20</v>
@@ -1316,7 +1294,7 @@
         <v>6.2</v>
       </c>
       <c r="N15" s="7">
-        <v>12.65</v>
+        <v>12.4</v>
       </c>
       <c r="O15" s="8" t="s">
         <v>20</v>
@@ -1335,35 +1313,35 @@
       <c r="D16" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E16" s="16">
+      <c r="E16" s="10">
         <v>0.11</v>
       </c>
-      <c r="F16" s="17">
+      <c r="F16" s="16">
         <v>0.11799999999999999</v>
       </c>
-      <c r="G16" s="18">
+      <c r="G16" s="12">
         <v>0.11</v>
       </c>
-      <c r="H16" s="18">
+      <c r="H16" s="12">
         <v>0.11</v>
       </c>
-      <c r="I16" s="18">
+      <c r="I16" s="12">
         <v>0.11</v>
       </c>
-      <c r="J16" s="19">
+      <c r="J16" s="15">
         <v>0.16200000000000001</v>
       </c>
-      <c r="K16" s="20">
-        <v>0.155</v>
+      <c r="K16" s="14">
+        <v>0.152</v>
       </c>
       <c r="L16" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="M16" s="19">
+      <c r="M16" s="15">
         <v>6.1499999999999999E-2</v>
       </c>
-      <c r="N16" s="20">
-        <v>0.155</v>
+      <c r="N16" s="14">
+        <v>0.152</v>
       </c>
       <c r="O16" s="8" t="s">
         <v>20</v>
@@ -1382,35 +1360,35 @@
       <c r="D17" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E17" s="16">
+      <c r="E17" s="10">
         <v>0.19969999999999999</v>
       </c>
-      <c r="F17" s="17">
+      <c r="F17" s="16">
         <v>0.25900000000000001</v>
       </c>
-      <c r="G17" s="18">
+      <c r="G17" s="12">
         <v>0.19969999999999999</v>
       </c>
-      <c r="H17" s="18">
+      <c r="H17" s="12">
         <v>0.19969999999999999</v>
       </c>
-      <c r="I17" s="18">
+      <c r="I17" s="12">
         <v>0.19969999999999999</v>
       </c>
-      <c r="J17" s="19">
+      <c r="J17" s="15">
         <v>0.35599999999999998</v>
       </c>
-      <c r="K17" s="20">
-        <v>0.35</v>
+      <c r="K17" s="14">
+        <v>0.40400000000000003</v>
       </c>
       <c r="L17" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="M17" s="19">
+      <c r="M17" s="15">
         <v>0.13</v>
       </c>
-      <c r="N17" s="20">
-        <v>0.35</v>
+      <c r="N17" s="14">
+        <v>0.40400000000000003</v>
       </c>
       <c r="O17" s="8" t="s">
         <v>20</v>
@@ -1429,35 +1407,35 @@
       <c r="D18" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E18" s="16">
+      <c r="E18" s="10">
         <v>0.20150000000000001</v>
       </c>
-      <c r="F18" s="21">
+      <c r="F18" s="11">
         <v>0.20150000000000001</v>
       </c>
-      <c r="G18" s="18">
+      <c r="G18" s="12">
         <v>0.20150000000000001</v>
       </c>
-      <c r="H18" s="18">
+      <c r="H18" s="12">
         <v>0.20150000000000001</v>
       </c>
-      <c r="I18" s="18">
+      <c r="I18" s="12">
         <v>0.20150000000000001</v>
       </c>
-      <c r="J18" s="19">
+      <c r="J18" s="15">
         <v>0.32900000000000001</v>
       </c>
-      <c r="K18" s="20">
-        <v>0.25</v>
+      <c r="K18" s="14">
+        <v>0.24299999999999999</v>
       </c>
       <c r="L18" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="M18" s="19">
+      <c r="M18" s="15">
         <v>0.1009</v>
       </c>
-      <c r="N18" s="20">
-        <v>0.25</v>
+      <c r="N18" s="14">
+        <v>0.24299999999999999</v>
       </c>
       <c r="O18" s="8" t="s">
         <v>20</v>
@@ -1476,35 +1454,35 @@
       <c r="D19" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E19" s="16">
+      <c r="E19" s="10">
         <v>0.2233</v>
       </c>
-      <c r="F19" s="17">
+      <c r="F19" s="16">
         <v>0.34599999999999997</v>
       </c>
-      <c r="G19" s="18">
+      <c r="G19" s="12">
         <v>0.2233</v>
       </c>
-      <c r="H19" s="18">
+      <c r="H19" s="12">
         <v>0.2233</v>
       </c>
-      <c r="I19" s="20">
+      <c r="I19" s="14">
         <v>0.23300000000000001</v>
       </c>
-      <c r="J19" s="19">
+      <c r="J19" s="15">
         <v>0.36499999999999999</v>
       </c>
-      <c r="K19" s="20">
-        <v>0.35</v>
+      <c r="K19" s="14">
+        <v>0.36899999999999999</v>
       </c>
       <c r="L19" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="M19" s="19">
+      <c r="M19" s="15">
         <v>0.14000000000000001</v>
       </c>
-      <c r="N19" s="20">
-        <v>0.35</v>
+      <c r="N19" s="14">
+        <v>0.36899999999999999</v>
       </c>
       <c r="O19" s="8" t="s">
         <v>20</v>
@@ -1523,35 +1501,35 @@
       <c r="D20" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E20" s="16">
+      <c r="E20" s="10">
         <v>0.19040000000000001</v>
       </c>
-      <c r="F20" s="17">
+      <c r="F20" s="16">
         <v>0.254</v>
       </c>
-      <c r="G20" s="20">
+      <c r="G20" s="14">
         <v>0.215</v>
       </c>
-      <c r="H20" s="18">
+      <c r="H20" s="12">
         <v>0.19040000000000001</v>
       </c>
-      <c r="I20" s="20">
+      <c r="I20" s="14">
         <v>0.20200000000000001</v>
       </c>
-      <c r="J20" s="19">
+      <c r="J20" s="15">
         <v>0.33300000000000002</v>
       </c>
-      <c r="K20" s="20">
-        <v>0.33</v>
+      <c r="K20" s="14">
+        <v>0.35699999999999998</v>
       </c>
       <c r="L20" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="M20" s="19">
+      <c r="M20" s="15">
         <v>0.1</v>
       </c>
-      <c r="N20" s="20">
-        <v>0.33</v>
+      <c r="N20" s="14">
+        <v>0.35699999999999998</v>
       </c>
       <c r="O20" s="8" t="s">
         <v>20</v>
@@ -1570,35 +1548,35 @@
       <c r="D21" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E21" s="16">
+      <c r="E21" s="10">
         <v>0.20150000000000001</v>
       </c>
-      <c r="F21" s="21">
+      <c r="F21" s="11">
         <v>0.20150000000000001</v>
       </c>
-      <c r="G21" s="18">
+      <c r="G21" s="12">
         <v>0.20150000000000001</v>
       </c>
-      <c r="H21" s="18">
+      <c r="H21" s="12">
         <v>0.20150000000000001</v>
       </c>
-      <c r="I21" s="20">
+      <c r="I21" s="14">
         <v>0.21299999999999999</v>
       </c>
-      <c r="J21" s="19">
+      <c r="J21" s="15">
         <v>0.32900000000000001</v>
       </c>
-      <c r="K21" s="20">
-        <v>0.19800000000000001</v>
+      <c r="K21" s="14">
+        <v>0.21199999999999999</v>
       </c>
       <c r="L21" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="M21" s="19">
+      <c r="M21" s="15">
         <v>0.1009</v>
       </c>
-      <c r="N21" s="20">
-        <v>0.19800000000000001</v>
+      <c r="N21" s="14">
+        <v>0.21199999999999999</v>
       </c>
       <c r="O21" s="8" t="s">
         <v>20</v>
@@ -1617,35 +1595,35 @@
       <c r="D22" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="E22" s="3">
+      <c r="E22" s="10">
         <v>11.284000000000001</v>
       </c>
-      <c r="F22" s="4">
+      <c r="F22" s="11">
         <v>11.284000000000001</v>
       </c>
-      <c r="G22" s="5">
+      <c r="G22" s="12">
         <v>11.284000000000001</v>
       </c>
-      <c r="H22" s="5">
+      <c r="H22" s="12">
         <v>11.284000000000001</v>
       </c>
-      <c r="I22" s="5">
+      <c r="I22" s="12">
         <v>11.284000000000001</v>
       </c>
-      <c r="J22" s="6">
+      <c r="J22" s="15">
         <v>25.9</v>
       </c>
-      <c r="K22" s="7">
-        <v>12.8</v>
+      <c r="K22" s="14">
+        <v>12.1</v>
       </c>
       <c r="L22" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="M22" s="6">
+      <c r="M22" s="15">
         <v>5.6504000000000003</v>
       </c>
-      <c r="N22" s="7">
-        <v>12.8</v>
+      <c r="N22" s="14">
+        <v>12.1</v>
       </c>
       <c r="O22" s="8" t="s">
         <v>20</v>
@@ -1664,35 +1642,35 @@
       <c r="D23" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E23" s="16">
+      <c r="E23" s="10">
         <v>0.23169999999999999</v>
       </c>
-      <c r="F23" s="17">
+      <c r="F23" s="16">
         <v>0.30199999999999999</v>
       </c>
-      <c r="G23" s="20">
+      <c r="G23" s="14">
         <v>0.28599999999999998</v>
       </c>
-      <c r="H23" s="20">
+      <c r="H23" s="14">
         <v>0.26600000000000001</v>
       </c>
-      <c r="I23" s="20">
+      <c r="I23" s="14">
         <v>0.26700000000000002</v>
       </c>
-      <c r="J23" s="19">
+      <c r="J23" s="15">
         <v>0.311</v>
       </c>
-      <c r="K23" s="20">
-        <v>0.28000000000000003</v>
+      <c r="K23" s="14">
+        <v>0.57899999999999996</v>
       </c>
       <c r="L23" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="M23" s="19">
+      <c r="M23" s="15">
         <v>0.1009</v>
       </c>
-      <c r="N23" s="20">
-        <v>0.28000000000000003</v>
+      <c r="N23" s="14">
+        <v>0.57899999999999996</v>
       </c>
       <c r="O23" s="8" t="s">
         <v>20</v>
@@ -1711,35 +1689,35 @@
       <c r="D24" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E24" s="16">
+      <c r="E24" s="10">
         <v>0.20150000000000001</v>
       </c>
-      <c r="F24" s="21">
+      <c r="F24" s="11">
         <v>0.20150000000000001</v>
       </c>
-      <c r="G24" s="18">
+      <c r="G24" s="12">
         <v>0.20150000000000001</v>
       </c>
-      <c r="H24" s="20">
+      <c r="H24" s="14">
         <v>0.20200000000000001</v>
       </c>
-      <c r="I24" s="20">
+      <c r="I24" s="14">
         <v>0.22600000000000001</v>
       </c>
-      <c r="J24" s="22">
+      <c r="J24" s="13">
         <v>0.20150000000000001</v>
       </c>
-      <c r="K24" s="20">
-        <v>0.19</v>
+      <c r="K24" s="14">
+        <v>0.2</v>
       </c>
       <c r="L24" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="M24" s="19">
+      <c r="M24" s="15">
         <v>0.1009</v>
       </c>
-      <c r="N24" s="20">
-        <v>0.19</v>
+      <c r="N24" s="14">
+        <v>0.2</v>
       </c>
       <c r="O24" s="8" t="s">
         <v>20</v>
@@ -1758,35 +1736,35 @@
       <c r="D25" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E25" s="16">
+      <c r="E25" s="10">
         <v>0.20150000000000001</v>
       </c>
-      <c r="F25" s="21">
+      <c r="F25" s="11">
         <v>0.20150000000000001</v>
       </c>
-      <c r="G25" s="20">
+      <c r="G25" s="14">
         <v>0.20300000000000001</v>
       </c>
-      <c r="H25" s="18">
+      <c r="H25" s="12">
         <v>0.20150000000000001</v>
       </c>
-      <c r="I25" s="20">
+      <c r="I25" s="14">
         <v>0.215</v>
       </c>
-      <c r="J25" s="19">
+      <c r="J25" s="15">
         <v>0.255</v>
       </c>
-      <c r="K25" s="20">
-        <v>0.20499999999999999</v>
+      <c r="K25" s="14">
+        <v>0.36</v>
       </c>
       <c r="L25" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="M25" s="19">
+      <c r="M25" s="15">
         <v>0.1009</v>
       </c>
-      <c r="N25" s="20">
-        <v>0.20499999999999999</v>
+      <c r="N25" s="14">
+        <v>0.36</v>
       </c>
       <c r="O25" s="8" t="s">
         <v>20</v>
@@ -1805,35 +1783,35 @@
       <c r="D26" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E26" s="16">
+      <c r="E26" s="10">
         <v>0.20150000000000001</v>
       </c>
-      <c r="F26" s="17">
+      <c r="F26" s="16">
         <v>0.23</v>
       </c>
-      <c r="G26" s="20">
+      <c r="G26" s="14">
         <v>0.222</v>
       </c>
-      <c r="H26" s="20">
+      <c r="H26" s="14">
         <v>0.24199999999999999</v>
       </c>
-      <c r="I26" s="20">
+      <c r="I26" s="14">
         <v>0.27100000000000002</v>
       </c>
-      <c r="J26" s="19">
+      <c r="J26" s="15">
         <v>0.22600000000000001</v>
       </c>
-      <c r="K26" s="20">
-        <v>0.22800000000000001</v>
+      <c r="K26" s="14">
+        <v>0.24</v>
       </c>
       <c r="L26" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="M26" s="19">
+      <c r="M26" s="15">
         <v>0.1009</v>
       </c>
-      <c r="N26" s="20">
-        <v>0.22800000000000001</v>
+      <c r="N26" s="14">
+        <v>0.24</v>
       </c>
       <c r="O26" s="8" t="s">
         <v>20</v>
@@ -1852,35 +1830,35 @@
       <c r="D27" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E27" s="16">
+      <c r="E27" s="10">
         <v>0.23169999999999999</v>
       </c>
-      <c r="F27" s="17">
+      <c r="F27" s="16">
         <v>0.34</v>
       </c>
-      <c r="G27" s="20">
+      <c r="G27" s="14">
         <v>0.35</v>
       </c>
-      <c r="H27" s="20">
+      <c r="H27" s="14">
         <v>0.37</v>
       </c>
-      <c r="I27" s="20">
+      <c r="I27" s="14">
         <v>0.37</v>
       </c>
-      <c r="J27" s="19">
+      <c r="J27" s="15">
         <v>0.39</v>
       </c>
-      <c r="K27" s="20">
-        <v>0.41</v>
+      <c r="K27" s="14">
+        <v>0.4</v>
       </c>
       <c r="L27" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="M27" s="19">
+      <c r="M27" s="15">
         <v>0.1009</v>
       </c>
-      <c r="N27" s="20">
-        <v>0.41</v>
+      <c r="N27" s="14">
+        <v>0.4</v>
       </c>
       <c r="O27" s="8" t="s">
         <v>20</v>
@@ -1899,35 +1877,35 @@
       <c r="D28" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E28" s="16">
+      <c r="E28" s="10">
         <v>0.36699999999999999</v>
       </c>
-      <c r="F28" s="21">
+      <c r="F28" s="11">
         <v>0.36699999999999999</v>
       </c>
-      <c r="G28" s="18">
+      <c r="G28" s="12">
         <v>0.36699999999999999</v>
       </c>
-      <c r="H28" s="18">
+      <c r="H28" s="12">
         <v>0.36699999999999999</v>
       </c>
-      <c r="I28" s="18">
+      <c r="I28" s="12">
         <v>0.36699999999999999</v>
       </c>
-      <c r="J28" s="19">
+      <c r="J28" s="15">
         <v>0.46750000000000003</v>
       </c>
-      <c r="K28" s="20">
-        <v>0.3982</v>
+      <c r="K28" s="14">
+        <v>0.39489999999999997</v>
       </c>
       <c r="L28" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="M28" s="19">
+      <c r="M28" s="15">
         <v>0.25</v>
       </c>
-      <c r="N28" s="20">
-        <v>0.3982</v>
+      <c r="N28" s="14">
+        <v>0.39489999999999997</v>
       </c>
       <c r="O28" s="8" t="s">
         <v>20</v>
@@ -1946,35 +1924,35 @@
       <c r="D29" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E29" s="16">
+      <c r="E29" s="10">
         <v>0.14000000000000001</v>
       </c>
-      <c r="F29" s="21">
+      <c r="F29" s="11">
         <v>0.14000000000000001</v>
       </c>
-      <c r="G29" s="18">
+      <c r="G29" s="12">
         <v>0.14000000000000001</v>
       </c>
-      <c r="H29" s="18">
+      <c r="H29" s="12">
         <v>0.14000000000000001</v>
       </c>
-      <c r="I29" s="18">
+      <c r="I29" s="12">
         <v>0.14000000000000001</v>
       </c>
-      <c r="J29" s="22">
+      <c r="J29" s="13">
         <v>0.14000000000000001</v>
       </c>
-      <c r="K29" s="20">
-        <v>0.16</v>
+      <c r="K29" s="14">
+        <v>0.159</v>
       </c>
       <c r="L29" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="M29" s="19">
+      <c r="M29" s="15">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="N29" s="20">
-        <v>0.16</v>
+      <c r="N29" s="14">
+        <v>0.159</v>
       </c>
       <c r="O29" s="8" t="s">
         <v>20</v>
@@ -1993,219 +1971,219 @@
       <c r="D30" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E30" s="16">
+      <c r="E30" s="10">
         <v>0.14000000000000001</v>
       </c>
-      <c r="F30" s="21">
+      <c r="F30" s="11">
         <v>0.14000000000000001</v>
       </c>
-      <c r="G30" s="18">
+      <c r="G30" s="12">
         <v>0.14000000000000001</v>
       </c>
-      <c r="H30" s="18">
+      <c r="H30" s="12">
         <v>0.14000000000000001</v>
       </c>
-      <c r="I30" s="18">
+      <c r="I30" s="12">
         <v>0.14000000000000001</v>
       </c>
-      <c r="J30" s="22">
+      <c r="J30" s="13">
         <v>0.14000000000000001</v>
       </c>
-      <c r="K30" s="20">
-        <v>0.17499999999999999</v>
+      <c r="K30" s="14">
+        <v>0.17199999999999999</v>
       </c>
       <c r="L30" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="M30" s="19">
+      <c r="M30" s="15">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="N30" s="20">
-        <v>0.17499999999999999</v>
+      <c r="N30" s="14">
+        <v>0.17199999999999999</v>
       </c>
       <c r="O30" s="8" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="31" spans="1:15" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="23" t="s">
+      <c r="A31" s="17" t="s">
         <v>50</v>
       </c>
-      <c r="B31" s="24" t="s">
+      <c r="B31" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="C31" s="24" t="s">
+      <c r="C31" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="D31" s="24" t="s">
+      <c r="D31" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="E31" s="25">
+      <c r="E31" s="19">
         <v>0.185</v>
       </c>
-      <c r="F31" s="26">
+      <c r="F31" s="20">
         <v>0.20100000000000001</v>
       </c>
-      <c r="G31" s="27">
+      <c r="G31" s="21">
         <v>0.21099999999999999</v>
       </c>
-      <c r="H31" s="27">
+      <c r="H31" s="21">
         <v>0.216</v>
       </c>
-      <c r="I31" s="27">
+      <c r="I31" s="21">
         <v>0.22600000000000001</v>
       </c>
-      <c r="J31" s="28">
+      <c r="J31" s="22">
         <v>0.31900000000000001</v>
       </c>
-      <c r="K31" s="27">
-        <v>0.3</v>
-      </c>
-      <c r="L31" s="29" t="s">
-        <v>20</v>
-      </c>
-      <c r="M31" s="28">
+      <c r="K31" s="21">
+        <v>0.223</v>
+      </c>
+      <c r="L31" s="23" t="s">
+        <v>20</v>
+      </c>
+      <c r="M31" s="22">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="N31" s="27">
-        <v>0.3</v>
-      </c>
-      <c r="O31" s="29" t="s">
+      <c r="N31" s="21">
+        <v>0.223</v>
+      </c>
+      <c r="O31" s="23" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="33" spans="1:15" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="32" t="s">
+      <c r="A33" s="26" t="s">
         <v>53</v>
       </c>
-      <c r="B33" s="32"/>
-      <c r="C33" s="32"/>
-      <c r="D33" s="32"/>
-      <c r="E33" s="32"/>
-      <c r="F33" s="32"/>
-      <c r="G33" s="32"/>
-      <c r="H33" s="32"/>
-      <c r="I33" s="32"/>
-      <c r="J33" s="32"/>
-      <c r="K33" s="32"/>
-      <c r="L33" s="32"/>
-      <c r="M33" s="32"/>
-      <c r="N33" s="32"/>
-      <c r="O33" s="32"/>
+      <c r="B33" s="26"/>
+      <c r="C33" s="26"/>
+      <c r="D33" s="26"/>
+      <c r="E33" s="26"/>
+      <c r="F33" s="26"/>
+      <c r="G33" s="26"/>
+      <c r="H33" s="26"/>
+      <c r="I33" s="26"/>
+      <c r="J33" s="26"/>
+      <c r="K33" s="26"/>
+      <c r="L33" s="26"/>
+      <c r="M33" s="26"/>
+      <c r="N33" s="26"/>
+      <c r="O33" s="26"/>
     </row>
     <row r="34" spans="1:15" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="32" t="s">
+      <c r="A34" s="26" t="s">
         <v>54</v>
       </c>
-      <c r="B34" s="32"/>
-      <c r="C34" s="32"/>
-      <c r="D34" s="32"/>
-      <c r="E34" s="32"/>
-      <c r="F34" s="32"/>
-      <c r="G34" s="32"/>
-      <c r="H34" s="32"/>
-      <c r="I34" s="32"/>
-      <c r="J34" s="32"/>
-      <c r="K34" s="32"/>
-      <c r="L34" s="32"/>
-      <c r="M34" s="32"/>
-      <c r="N34" s="32"/>
-      <c r="O34" s="32"/>
+      <c r="B34" s="26"/>
+      <c r="C34" s="26"/>
+      <c r="D34" s="26"/>
+      <c r="E34" s="26"/>
+      <c r="F34" s="26"/>
+      <c r="G34" s="26"/>
+      <c r="H34" s="26"/>
+      <c r="I34" s="26"/>
+      <c r="J34" s="26"/>
+      <c r="K34" s="26"/>
+      <c r="L34" s="26"/>
+      <c r="M34" s="26"/>
+      <c r="N34" s="26"/>
+      <c r="O34" s="26"/>
     </row>
     <row r="35" spans="1:15" ht="26.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="32" t="s">
+      <c r="A35" s="26" t="s">
         <v>55</v>
       </c>
-      <c r="B35" s="32"/>
-      <c r="C35" s="32"/>
-      <c r="D35" s="32"/>
-      <c r="E35" s="32"/>
-      <c r="F35" s="32"/>
-      <c r="G35" s="32"/>
-      <c r="H35" s="32"/>
-      <c r="I35" s="32"/>
-      <c r="J35" s="32"/>
-      <c r="K35" s="32"/>
-      <c r="L35" s="32"/>
-      <c r="M35" s="32"/>
-      <c r="N35" s="32"/>
-      <c r="O35" s="32"/>
+      <c r="B35" s="26"/>
+      <c r="C35" s="26"/>
+      <c r="D35" s="26"/>
+      <c r="E35" s="26"/>
+      <c r="F35" s="26"/>
+      <c r="G35" s="26"/>
+      <c r="H35" s="26"/>
+      <c r="I35" s="26"/>
+      <c r="J35" s="26"/>
+      <c r="K35" s="26"/>
+      <c r="L35" s="26"/>
+      <c r="M35" s="26"/>
+      <c r="N35" s="26"/>
+      <c r="O35" s="26"/>
     </row>
     <row r="36" spans="1:15" ht="26.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="32" t="s">
+      <c r="A36" s="26" t="s">
         <v>56</v>
       </c>
-      <c r="B36" s="32"/>
-      <c r="C36" s="32"/>
-      <c r="D36" s="32"/>
-      <c r="E36" s="32"/>
-      <c r="F36" s="32"/>
-      <c r="G36" s="32"/>
-      <c r="H36" s="32"/>
-      <c r="I36" s="32"/>
-      <c r="J36" s="32"/>
-      <c r="K36" s="32"/>
-      <c r="L36" s="32"/>
-      <c r="M36" s="32"/>
-      <c r="N36" s="32"/>
-      <c r="O36" s="32"/>
+      <c r="B36" s="26"/>
+      <c r="C36" s="26"/>
+      <c r="D36" s="26"/>
+      <c r="E36" s="26"/>
+      <c r="F36" s="26"/>
+      <c r="G36" s="26"/>
+      <c r="H36" s="26"/>
+      <c r="I36" s="26"/>
+      <c r="J36" s="26"/>
+      <c r="K36" s="26"/>
+      <c r="L36" s="26"/>
+      <c r="M36" s="26"/>
+      <c r="N36" s="26"/>
+      <c r="O36" s="26"/>
     </row>
     <row r="37" spans="1:15" ht="26.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="32" t="s">
+      <c r="A37" s="26" t="s">
         <v>57</v>
       </c>
-      <c r="B37" s="32"/>
-      <c r="C37" s="32"/>
-      <c r="D37" s="32"/>
-      <c r="E37" s="32"/>
-      <c r="F37" s="32"/>
-      <c r="G37" s="32"/>
-      <c r="H37" s="32"/>
-      <c r="I37" s="32"/>
-      <c r="J37" s="32"/>
-      <c r="K37" s="32"/>
-      <c r="L37" s="32"/>
-      <c r="M37" s="32"/>
-      <c r="N37" s="32"/>
-      <c r="O37" s="32"/>
+      <c r="B37" s="26"/>
+      <c r="C37" s="26"/>
+      <c r="D37" s="26"/>
+      <c r="E37" s="26"/>
+      <c r="F37" s="26"/>
+      <c r="G37" s="26"/>
+      <c r="H37" s="26"/>
+      <c r="I37" s="26"/>
+      <c r="J37" s="26"/>
+      <c r="K37" s="26"/>
+      <c r="L37" s="26"/>
+      <c r="M37" s="26"/>
+      <c r="N37" s="26"/>
+      <c r="O37" s="26"/>
     </row>
     <row r="38" spans="1:15" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="32" t="s">
+      <c r="A38" s="26" t="s">
         <v>58</v>
       </c>
-      <c r="B38" s="32"/>
-      <c r="C38" s="32"/>
-      <c r="D38" s="32"/>
-      <c r="E38" s="32"/>
-      <c r="F38" s="32"/>
-      <c r="G38" s="32"/>
-      <c r="H38" s="32"/>
-      <c r="I38" s="32"/>
-      <c r="J38" s="32"/>
-      <c r="K38" s="32"/>
-      <c r="L38" s="32"/>
-      <c r="M38" s="32"/>
-      <c r="N38" s="32"/>
-      <c r="O38" s="32"/>
+      <c r="B38" s="26"/>
+      <c r="C38" s="26"/>
+      <c r="D38" s="26"/>
+      <c r="E38" s="26"/>
+      <c r="F38" s="26"/>
+      <c r="G38" s="26"/>
+      <c r="H38" s="26"/>
+      <c r="I38" s="26"/>
+      <c r="J38" s="26"/>
+      <c r="K38" s="26"/>
+      <c r="L38" s="26"/>
+      <c r="M38" s="26"/>
+      <c r="N38" s="26"/>
+      <c r="O38" s="26"/>
     </row>
     <row r="39" spans="1:15" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="32" t="s">
+      <c r="A39" s="26" t="s">
         <v>59</v>
       </c>
-      <c r="B39" s="32"/>
-      <c r="C39" s="32"/>
-      <c r="D39" s="32"/>
-      <c r="E39" s="32"/>
-      <c r="F39" s="32"/>
-      <c r="G39" s="32"/>
-      <c r="H39" s="32"/>
-      <c r="I39" s="32"/>
-      <c r="J39" s="32"/>
-      <c r="K39" s="32"/>
-      <c r="L39" s="32"/>
-      <c r="M39" s="32"/>
-      <c r="N39" s="32"/>
-      <c r="O39" s="32"/>
+      <c r="B39" s="26"/>
+      <c r="C39" s="26"/>
+      <c r="D39" s="26"/>
+      <c r="E39" s="26"/>
+      <c r="F39" s="26"/>
+      <c r="G39" s="26"/>
+      <c r="H39" s="26"/>
+      <c r="I39" s="26"/>
+      <c r="J39" s="26"/>
+      <c r="K39" s="26"/>
+      <c r="L39" s="26"/>
+      <c r="M39" s="26"/>
+      <c r="N39" s="26"/>
+      <c r="O39" s="26"/>
     </row>
   </sheetData>
   <mergeCells count="34">

</xml_diff>